<commit_message>
Add RecipientSignature and RecipientPhoto on delivered import
</commit_message>
<xml_diff>
--- a/client/assets/template/importMarkAsDelivered.xlsx
+++ b/client/assets/template/importMarkAsDelivered.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fadhil I\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\etobee-admin\client\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>RecipientName</t>
   </si>
@@ -39,18 +39,32 @@
   </si>
   <si>
     <t>EDSNumber</t>
+  </si>
+  <si>
+    <t>RecipientSignature</t>
+  </si>
+  <si>
+    <t>RecipientPhoto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="1"/>
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
@@ -75,8 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,22 +374,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="7" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -388,6 +402,15 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>